<commit_message>
Changed picture in index
</commit_message>
<xml_diff>
--- a/exceltocsv/public/reports/employee dtr/Ardamoy,Ma. Rica Catherine.xlsx
+++ b/exceltocsv/public/reports/employee dtr/Ardamoy,Ma. Rica Catherine.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="74" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="74" xml:space="preserve">
   <si>
     <t>iRipple, Inc.</t>
   </si>
@@ -613,7 +613,9 @@
       <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>

</xml_diff>